<commit_message>
mise a jour mardi
</commit_message>
<xml_diff>
--- a/TestsFonctionnelsProjetFinal.xlsx
+++ b/TestsFonctionnelsProjetFinal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joach\Desktop\ProjetFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3782659-3B06-467D-93FD-1F281ABAA4A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877E8CCD-5BCE-4B3B-A764-C1015F32D2AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{981B120D-79F7-4D01-A47B-1890E44FAFDB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{981B120D-79F7-4D01-A47B-1890E44FAFDB}"/>
   </bookViews>
   <sheets>
     <sheet name="PageAuth" sheetId="6" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="101">
   <si>
     <t>Tests fonctionnels</t>
   </si>
@@ -189,27 +189,12 @@
     <t>Supprimer prospect</t>
   </si>
   <si>
-    <t>Bouton appeler + bouton retour</t>
-  </si>
-  <si>
-    <t>Bouton rdv + bouton retour</t>
-  </si>
-  <si>
-    <t>Ajouter prospect + bouton retour</t>
-  </si>
-  <si>
-    <t>Créer un contact + bouton retour</t>
-  </si>
-  <si>
     <t>Ajouter prospect csv</t>
   </si>
   <si>
     <t>Page admin</t>
   </si>
   <si>
-    <t>Accès espace personnel - Modifier password + bouton retour</t>
-  </si>
-  <si>
     <t>Afficher listes formations: en cours, à venir et finies</t>
   </si>
   <si>
@@ -219,9 +204,6 @@
     <t xml:space="preserve">Ajouter pdf formation </t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
     <t>Afficher listes prospects selon commercial et liste prospects sans commercial attribué</t>
   </si>
   <si>
@@ -343,6 +325,24 @@
   </si>
   <si>
     <t>Afficher contact associe</t>
+  </si>
+  <si>
+    <t>Bouton rdv</t>
+  </si>
+  <si>
+    <t>Ajouter prospect</t>
+  </si>
+  <si>
+    <t>Bouton appeler</t>
+  </si>
+  <si>
+    <t>Envoyer mail quand participant ajouter</t>
+  </si>
+  <si>
+    <t>Bouton relance + envoie email</t>
+  </si>
+  <si>
+    <t>Envoie mail</t>
   </si>
 </sst>
 </file>
@@ -690,6 +690,9 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -697,9 +700,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1030,14 +1030,14 @@
   </cols>
   <sheetData>
     <row r="5" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D5" s="51" t="s">
+      <c r="D5" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="54"/>
     </row>
     <row r="6" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D6" s="10" t="s">
@@ -1067,10 +1067,10 @@
         <v>7</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G7" s="26" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="H7" s="2">
         <v>1</v>
@@ -1084,7 +1084,7 @@
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
       <c r="G8" s="15" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H8" s="2">
         <v>1</v>
@@ -1098,12 +1098,12 @@
       <c r="E9" s="33"/>
       <c r="F9" s="31"/>
       <c r="G9" s="44" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H9" s="30">
         <v>1</v>
       </c>
-      <c r="I9" s="54"/>
+      <c r="I9" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1186,8 +1186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42B5DE11-A17A-4527-9F20-476B372D9BD6}">
   <dimension ref="D1:K21"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1214,14 +1214,14 @@
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D5" s="51" t="s">
+      <c r="D5" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="54"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
     </row>
@@ -1258,7 +1258,7 @@
         <v>3</v>
       </c>
       <c r="G7" s="45" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="H7" s="2">
         <v>1</v>
@@ -1333,7 +1333,7 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="4:11" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D12" s="9">
         <v>6</v>
       </c>
@@ -1343,9 +1343,11 @@
         <v>11</v>
       </c>
       <c r="H12" s="2">
-        <v>1</v>
-      </c>
-      <c r="I12" s="11"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="17" t="s">
+        <v>79</v>
+      </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
@@ -1358,10 +1360,12 @@
       <c r="G13" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="9">
-        <v>1</v>
-      </c>
-      <c r="I13" s="11"/>
+      <c r="H13" s="2">
+        <v>0</v>
+      </c>
+      <c r="I13" s="17" t="s">
+        <v>79</v>
+      </c>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
@@ -1453,7 +1457,7 @@
   <dimension ref="D5:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1467,14 +1471,14 @@
   </cols>
   <sheetData>
     <row r="5" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D5" s="51" t="s">
+      <c r="D5" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="54"/>
     </row>
     <row r="6" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D6" s="10" t="s">
@@ -1507,7 +1511,7 @@
         <v>16</v>
       </c>
       <c r="G7" s="26" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="H7" s="2">
         <v>1</v>
@@ -1521,7 +1525,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="15" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="H8" s="2">
         <v>1</v>
@@ -1566,9 +1570,11 @@
         <v>20</v>
       </c>
       <c r="H11" s="2">
-        <v>1</v>
-      </c>
-      <c r="I11" s="11"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="12" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D12" s="2">
@@ -1592,9 +1598,11 @@
         <v>21</v>
       </c>
       <c r="H13" s="2">
-        <v>1</v>
-      </c>
-      <c r="I13" s="11"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="17" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="14" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D14" s="2">
@@ -1645,9 +1653,11 @@
         <v>23</v>
       </c>
       <c r="H17" s="30">
-        <v>1</v>
-      </c>
-      <c r="I17" s="32"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="17" t="s">
+        <v>79</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1705,10 +1715,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F5AD64F-3C18-430E-9109-0A653C4C3160}">
-  <dimension ref="D5:K44"/>
+  <dimension ref="D5:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35:K36"/>
+    <sheetView topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1721,14 +1731,14 @@
   </cols>
   <sheetData>
     <row r="5" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D5" s="51" t="s">
+      <c r="D5" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="54"/>
     </row>
     <row r="6" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D6" s="10" t="s">
@@ -1761,7 +1771,7 @@
         <v>24</v>
       </c>
       <c r="G7" s="45" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="H7" s="2">
         <v>1</v>
@@ -1773,7 +1783,7 @@
         <v>2</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F8" s="19"/>
       <c r="G8" s="20" t="s">
@@ -1791,7 +1801,7 @@
       <c r="E9" s="19"/>
       <c r="F9" s="19"/>
       <c r="G9" s="21" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="H9" s="2">
         <v>1</v>
@@ -1819,7 +1829,7 @@
       <c r="E11" s="19"/>
       <c r="F11" s="19"/>
       <c r="G11" s="21" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="H11" s="2">
         <v>1</v>
@@ -1847,13 +1857,13 @@
       <c r="E13" s="19"/>
       <c r="F13" s="14"/>
       <c r="G13" s="20" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="H13" s="2">
         <v>0</v>
       </c>
       <c r="I13" s="25" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="4:9" x14ac:dyDescent="0.3">
@@ -1899,7 +1909,7 @@
       <c r="E17" s="19"/>
       <c r="F17" s="19"/>
       <c r="G17" s="21" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H17" s="2">
         <v>1</v>
@@ -1933,7 +1943,7 @@
         <v>0</v>
       </c>
       <c r="I19" s="25" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="4:9" x14ac:dyDescent="0.3">
@@ -1943,7 +1953,7 @@
       <c r="E20" s="19"/>
       <c r="F20" s="19"/>
       <c r="G20" s="21" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="H20" s="2">
         <v>1</v>
@@ -1957,7 +1967,7 @@
       <c r="E21" s="19"/>
       <c r="F21" s="19"/>
       <c r="G21" s="21" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="H21" s="2">
         <v>1</v>
@@ -2019,7 +2029,7 @@
         <v>0</v>
       </c>
       <c r="I25" s="25" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="4:9" x14ac:dyDescent="0.3">
@@ -2065,7 +2075,7 @@
       <c r="E29" s="19"/>
       <c r="F29" s="19"/>
       <c r="G29" s="21" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="H29" s="2">
         <v>1</v>
@@ -2099,7 +2109,7 @@
         <v>1</v>
       </c>
       <c r="I31" s="16" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" spans="4:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -2116,7 +2126,7 @@
       </c>
       <c r="I32" s="11"/>
     </row>
-    <row r="33" spans="4:11" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:9" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D33" s="9">
         <v>25</v>
       </c>
@@ -2130,7 +2140,7 @@
       </c>
       <c r="I33" s="11"/>
     </row>
-    <row r="34" spans="4:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D34" s="9">
         <v>26</v>
       </c>
@@ -2144,27 +2154,21 @@
       </c>
       <c r="I34" s="11"/>
     </row>
-    <row r="35" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D35" s="9">
         <v>27</v>
       </c>
       <c r="E35" s="19"/>
       <c r="F35" s="19"/>
       <c r="G35" s="20" t="s">
-        <v>18</v>
+        <v>99</v>
       </c>
       <c r="H35" s="2">
         <v>1</v>
       </c>
       <c r="I35" s="11"/>
-      <c r="J35" s="2">
-        <v>-2</v>
-      </c>
-      <c r="K35" s="16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="36" spans="4:11" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="4:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D36" s="9">
         <v>28</v>
       </c>
@@ -2177,124 +2181,161 @@
         <v>0</v>
       </c>
       <c r="I36" s="16" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="37" spans="4:11" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D37" s="9">
         <v>29</v>
       </c>
       <c r="E37" s="19"/>
       <c r="F37" s="19"/>
       <c r="G37" s="21" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="H37" s="2">
         <v>1</v>
       </c>
       <c r="I37" s="11"/>
     </row>
-    <row r="38" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D38" s="9">
         <v>30</v>
       </c>
       <c r="E38" s="19"/>
       <c r="F38" s="19"/>
       <c r="G38" s="21" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="H38" s="2">
         <v>1</v>
       </c>
       <c r="I38" s="11"/>
     </row>
-    <row r="39" spans="4:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D39" s="9">
         <v>31</v>
       </c>
       <c r="E39" s="19"/>
       <c r="F39" s="19"/>
       <c r="G39" s="21" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="H39" s="2">
-        <v>0</v>
-      </c>
-      <c r="I39" s="25" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="40" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D40" s="18"/>
+        <v>1</v>
+      </c>
+      <c r="I39" s="11"/>
+    </row>
+    <row r="40" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D40" s="9">
+        <v>32</v>
+      </c>
       <c r="E40" s="19"/>
       <c r="F40" s="19"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="18"/>
-      <c r="I40" s="18"/>
-    </row>
-    <row r="41" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D41" s="9">
-        <v>32</v>
-      </c>
+      <c r="G40" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="H40" s="2">
+        <v>0</v>
+      </c>
+      <c r="I40" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D41" s="18"/>
       <c r="E41" s="19"/>
       <c r="F41" s="19"/>
-      <c r="G41" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="H41" s="2">
-        <v>1</v>
-      </c>
-      <c r="I41" s="11"/>
-    </row>
-    <row r="42" spans="4:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G41" s="18"/>
+      <c r="H41" s="18"/>
+      <c r="I41" s="18"/>
+    </row>
+    <row r="42" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D42" s="9">
         <v>33</v>
       </c>
       <c r="E42" s="19"/>
       <c r="F42" s="19"/>
-      <c r="G42" s="17" t="s">
-        <v>45</v>
+      <c r="G42" s="22" t="s">
+        <v>9</v>
       </c>
       <c r="H42" s="2">
         <v>1</v>
       </c>
       <c r="I42" s="11"/>
     </row>
-    <row r="43" spans="4:11" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:9" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D43" s="9">
         <v>34</v>
       </c>
       <c r="E43" s="19"/>
       <c r="F43" s="19"/>
       <c r="G43" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="H43" s="2">
+        <v>1</v>
+      </c>
+      <c r="I43" s="11"/>
+    </row>
+    <row r="44" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D44" s="9">
+        <v>35</v>
+      </c>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="H43" s="2">
+      <c r="H44" s="2">
         <v>0</v>
       </c>
-      <c r="I43" s="25" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="44" spans="4:11" x14ac:dyDescent="0.3">
-      <c r="D44" s="43">
-        <v>35</v>
-      </c>
-      <c r="E44" s="42"/>
-      <c r="F44" s="42"/>
-      <c r="G44" s="35" t="s">
+      <c r="I44" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="45" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D45" s="43">
+        <v>36</v>
+      </c>
+      <c r="E45" s="42"/>
+      <c r="F45" s="42"/>
+      <c r="G45" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="H44" s="36">
-        <v>1</v>
-      </c>
-      <c r="I44" s="32"/>
+      <c r="H45" s="36">
+        <v>1</v>
+      </c>
+      <c r="I45" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D5:I5"/>
   </mergeCells>
   <conditionalFormatting sqref="H8">
+    <cfRule type="iconSet" priority="142">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="143">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0" gte="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="144">
+      <iconSet iconSet="3Signs">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H11">
     <cfRule type="iconSet" priority="139">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -2317,7 +2358,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H11">
+  <conditionalFormatting sqref="H9">
     <cfRule type="iconSet" priority="136">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -2340,7 +2381,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H9">
+  <conditionalFormatting sqref="H10">
     <cfRule type="iconSet" priority="133">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -2363,30 +2404,30 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H10">
-    <cfRule type="iconSet" priority="130">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="131">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0" gte="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="132">
-      <iconSet iconSet="3Signs">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="H12">
+    <cfRule type="iconSet" priority="126">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="127">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0" gte="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="128">
+      <iconSet iconSet="3Signs">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H13">
     <cfRule type="iconSet" priority="123">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -2409,38 +2450,15 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H13">
-    <cfRule type="iconSet" priority="120">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
+  <conditionalFormatting sqref="H45">
     <cfRule type="iconSet" priority="121">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0" gte="0"/>
+        <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
       </iconSet>
     </cfRule>
     <cfRule type="iconSet" priority="122">
-      <iconSet iconSet="3Signs">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H44">
-    <cfRule type="iconSet" priority="118">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="119">
       <iconSet iconSet="5Arrows">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="20"/>
@@ -2451,6 +2469,45 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
+    <cfRule type="iconSet" priority="91">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="92">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0" gte="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="93">
+      <iconSet iconSet="3Signs">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H45">
+    <cfRule type="iconSet" priority="219">
+      <iconSet iconSet="3Symbols2">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="220">
+      <iconSet iconSet="3Symbols2">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H15">
     <cfRule type="iconSet" priority="88">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -2473,498 +2530,597 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="H16">
+    <cfRule type="iconSet" priority="85">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="86">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0" gte="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="87">
+      <iconSet iconSet="3Signs">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H17">
+    <cfRule type="iconSet" priority="82">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="83">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0" gte="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="84">
+      <iconSet iconSet="3Signs">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H18">
+    <cfRule type="iconSet" priority="79">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="80">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0" gte="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="81">
+      <iconSet iconSet="3Signs">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H19">
+    <cfRule type="iconSet" priority="76">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="77">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0" gte="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="78">
+      <iconSet iconSet="3Signs">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H20">
+    <cfRule type="iconSet" priority="73">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="74">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0" gte="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="75">
+      <iconSet iconSet="3Signs">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H21">
+    <cfRule type="iconSet" priority="70">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="71">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0" gte="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="72">
+      <iconSet iconSet="3Signs">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H22">
+    <cfRule type="iconSet" priority="67">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="68">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0" gte="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="69">
+      <iconSet iconSet="3Signs">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H23">
+    <cfRule type="iconSet" priority="64">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="65">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0" gte="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="66">
+      <iconSet iconSet="3Signs">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H24">
+    <cfRule type="iconSet" priority="61">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="62">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0" gte="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="63">
+      <iconSet iconSet="3Signs">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H25">
+    <cfRule type="iconSet" priority="58">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="59">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0" gte="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="60">
+      <iconSet iconSet="3Signs">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H27">
+    <cfRule type="iconSet" priority="55">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="56">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0" gte="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="57">
+      <iconSet iconSet="3Signs">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H28">
+    <cfRule type="iconSet" priority="52">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="53">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0" gte="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="54">
+      <iconSet iconSet="3Signs">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H29">
+    <cfRule type="iconSet" priority="49">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="50">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0" gte="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="51">
+      <iconSet iconSet="3Signs">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H30">
+    <cfRule type="iconSet" priority="46">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="47">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0" gte="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="48">
+      <iconSet iconSet="3Signs">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H31">
+    <cfRule type="iconSet" priority="43">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="44">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0" gte="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="45">
+      <iconSet iconSet="3Signs">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H32">
+    <cfRule type="iconSet" priority="40">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="41">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0" gte="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="42">
+      <iconSet iconSet="3Signs">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H33">
+    <cfRule type="iconSet" priority="37">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="38">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0" gte="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="39">
+      <iconSet iconSet="3Signs">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H34">
+    <cfRule type="iconSet" priority="34">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="35">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0" gte="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="36">
+      <iconSet iconSet="3Signs">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H35">
+    <cfRule type="iconSet" priority="31">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="32">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0" gte="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="33">
+      <iconSet iconSet="3Signs">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H37">
+    <cfRule type="iconSet" priority="25">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="26">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0" gte="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="27">
+      <iconSet iconSet="3Signs">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H39">
+    <cfRule type="iconSet" priority="22">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="23">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0" gte="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="24">
+      <iconSet iconSet="3Signs">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H40">
+    <cfRule type="iconSet" priority="19">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="20">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0" gte="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="21">
+      <iconSet iconSet="3Signs">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H42">
+    <cfRule type="iconSet" priority="16">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="17">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0" gte="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="18">
+      <iconSet iconSet="3Signs">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H43">
+    <cfRule type="iconSet" priority="13">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="14">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0" gte="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="15">
+      <iconSet iconSet="3Signs">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="H44">
-    <cfRule type="iconSet" priority="216">
-      <iconSet iconSet="3Symbols2">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="217">
-      <iconSet iconSet="3Symbols2">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H15">
-    <cfRule type="iconSet" priority="85">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="86">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0" gte="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="87">
-      <iconSet iconSet="3Signs">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H16">
-    <cfRule type="iconSet" priority="82">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="83">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0" gte="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="84">
-      <iconSet iconSet="3Signs">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H17">
-    <cfRule type="iconSet" priority="79">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="80">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0" gte="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="81">
-      <iconSet iconSet="3Signs">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H18">
-    <cfRule type="iconSet" priority="76">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="77">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0" gte="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="78">
-      <iconSet iconSet="3Signs">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H19">
-    <cfRule type="iconSet" priority="73">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="74">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0" gte="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="75">
-      <iconSet iconSet="3Signs">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H20">
-    <cfRule type="iconSet" priority="70">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="71">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0" gte="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="72">
-      <iconSet iconSet="3Signs">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H21">
-    <cfRule type="iconSet" priority="67">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="68">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0" gte="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="69">
-      <iconSet iconSet="3Signs">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H22">
-    <cfRule type="iconSet" priority="64">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="65">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0" gte="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="66">
-      <iconSet iconSet="3Signs">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H23">
-    <cfRule type="iconSet" priority="61">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="62">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0" gte="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="63">
-      <iconSet iconSet="3Signs">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H24">
-    <cfRule type="iconSet" priority="58">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="59">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0" gte="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="60">
-      <iconSet iconSet="3Signs">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H25">
-    <cfRule type="iconSet" priority="55">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="56">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0" gte="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="57">
-      <iconSet iconSet="3Signs">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H27">
-    <cfRule type="iconSet" priority="52">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="53">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0" gte="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="54">
-      <iconSet iconSet="3Signs">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H28">
-    <cfRule type="iconSet" priority="49">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="50">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0" gte="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="51">
-      <iconSet iconSet="3Signs">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H29">
-    <cfRule type="iconSet" priority="46">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="47">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0" gte="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="48">
-      <iconSet iconSet="3Signs">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H30">
-    <cfRule type="iconSet" priority="43">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="44">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0" gte="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="45">
-      <iconSet iconSet="3Signs">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H31">
-    <cfRule type="iconSet" priority="40">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="41">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0" gte="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="42">
-      <iconSet iconSet="3Signs">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H32">
-    <cfRule type="iconSet" priority="37">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="38">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0" gte="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="39">
-      <iconSet iconSet="3Signs">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H33">
-    <cfRule type="iconSet" priority="34">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="35">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0" gte="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="36">
-      <iconSet iconSet="3Signs">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H34">
-    <cfRule type="iconSet" priority="31">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="32">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0" gte="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="33">
-      <iconSet iconSet="3Signs">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H35">
-    <cfRule type="iconSet" priority="28">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="29">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0" gte="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="30">
-      <iconSet iconSet="3Signs">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H37">
-    <cfRule type="iconSet" priority="22">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="23">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0" gte="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="24">
+    <cfRule type="iconSet" priority="10">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="11">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0" gte="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="12">
+      <iconSet iconSet="3Signs">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H36">
+    <cfRule type="iconSet" priority="4">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="5">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0" gte="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="6">
       <iconSet iconSet="3Signs">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -2973,144 +3129,6 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38">
-    <cfRule type="iconSet" priority="19">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="20">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0" gte="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="21">
-      <iconSet iconSet="3Signs">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H39">
-    <cfRule type="iconSet" priority="16">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="17">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0" gte="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="18">
-      <iconSet iconSet="3Signs">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H41">
-    <cfRule type="iconSet" priority="13">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="14">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0" gte="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="15">
-      <iconSet iconSet="3Signs">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H42">
-    <cfRule type="iconSet" priority="10">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="11">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0" gte="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="12">
-      <iconSet iconSet="3Signs">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H43">
-    <cfRule type="iconSet" priority="7">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="8">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0" gte="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="9">
-      <iconSet iconSet="3Signs">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J35">
-    <cfRule type="iconSet" priority="4">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="5">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0" gte="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="6">
-      <iconSet iconSet="3Signs">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H36">
     <cfRule type="iconSet" priority="1">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -3141,8 +3159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46D20008-74A7-4DFB-AE1C-7903EED8FBEE}">
   <dimension ref="D5:K24"/>
   <sheetViews>
-    <sheetView topLeftCell="E19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3194,7 +3212,7 @@
         <v>47</v>
       </c>
       <c r="G7" s="26" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="H7" s="2">
         <v>1</v>
@@ -3208,7 +3226,7 @@
       <c r="E8" s="13"/>
       <c r="F8" s="27"/>
       <c r="G8" s="25" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="H8" s="2">
         <v>1</v>
@@ -3236,7 +3254,7 @@
       <c r="E10" s="13"/>
       <c r="F10" s="27"/>
       <c r="G10" s="25" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="H10" s="2">
         <v>1</v>
@@ -3250,7 +3268,7 @@
       <c r="E11" s="13"/>
       <c r="F11" s="27"/>
       <c r="G11" s="25" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="H11" s="2">
         <v>1</v>
@@ -3264,7 +3282,7 @@
       <c r="E12" s="13"/>
       <c r="F12" s="27"/>
       <c r="G12" s="25" t="s">
-        <v>49</v>
+        <v>97</v>
       </c>
       <c r="H12" s="2">
         <v>1</v>
@@ -3278,17 +3296,17 @@
       <c r="E13" s="13"/>
       <c r="F13" s="27"/>
       <c r="G13" s="25" t="s">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="H13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I13" s="11"/>
-      <c r="J13" s="24">
-        <v>-2</v>
-      </c>
-      <c r="K13" s="16" t="s">
-        <v>59</v>
+      <c r="J13" s="2">
+        <v>-1</v>
+      </c>
+      <c r="K13" s="14" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="4:11" x14ac:dyDescent="0.3">
@@ -3298,7 +3316,7 @@
       <c r="E14" s="13"/>
       <c r="F14" s="27"/>
       <c r="G14" s="25" t="s">
-        <v>51</v>
+        <v>96</v>
       </c>
       <c r="H14" s="2">
         <v>1</v>
@@ -3312,7 +3330,7 @@
       <c r="E15" s="13"/>
       <c r="F15" s="27"/>
       <c r="G15" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="H15" s="2">
         <v>1</v>
@@ -3325,7 +3343,7 @@
       </c>
       <c r="E16" s="19"/>
       <c r="G16" s="25" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="H16" s="2">
         <v>1</v>
@@ -3345,7 +3363,7 @@
       </c>
       <c r="E18" s="19"/>
       <c r="G18" s="29" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="H18" s="2">
         <v>1</v>
@@ -3359,7 +3377,7 @@
       <c r="E19" s="13"/>
       <c r="F19" s="27"/>
       <c r="G19" s="29" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="H19" s="2">
         <v>1</v>
@@ -3395,7 +3413,7 @@
       <c r="E22" s="13"/>
       <c r="F22" s="27"/>
       <c r="G22" s="17" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="H22" s="2">
         <v>1</v>
@@ -3412,9 +3430,11 @@
         <v>23</v>
       </c>
       <c r="H23" s="2">
-        <v>1</v>
-      </c>
-      <c r="I23" s="11"/>
+        <v>0</v>
+      </c>
+      <c r="I23" s="16" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="24" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D24" s="40">
@@ -3432,14 +3452,14 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H8:H15">
-    <cfRule type="iconSet" priority="47">
+    <cfRule type="iconSet" priority="51">
       <iconSet iconSet="3Symbols2">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
       </iconSet>
     </cfRule>
-    <cfRule type="iconSet" priority="48">
+    <cfRule type="iconSet" priority="52">
       <iconSet iconSet="3Symbols2">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -3448,14 +3468,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8:H15">
-    <cfRule type="iconSet" priority="45">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="46">
+    <cfRule type="iconSet" priority="49">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="50">
       <iconSet iconSet="5Arrows">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="20"/>
@@ -3466,14 +3486,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23">
-    <cfRule type="iconSet" priority="43">
+    <cfRule type="iconSet" priority="47">
       <iconSet iconSet="3Symbols2">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
       </iconSet>
     </cfRule>
-    <cfRule type="iconSet" priority="44">
+    <cfRule type="iconSet" priority="48">
       <iconSet iconSet="3Symbols2">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -3482,14 +3502,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H23">
-    <cfRule type="iconSet" priority="41">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="42">
+    <cfRule type="iconSet" priority="45">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="46">
       <iconSet iconSet="5Arrows">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="20"/>
@@ -3500,14 +3520,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="iconSet" priority="39">
+    <cfRule type="iconSet" priority="43">
       <iconSet iconSet="3Symbols2">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
       </iconSet>
     </cfRule>
-    <cfRule type="iconSet" priority="40">
+    <cfRule type="iconSet" priority="44">
       <iconSet iconSet="3Symbols2">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -3516,14 +3536,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H24">
-    <cfRule type="iconSet" priority="37">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="38">
+    <cfRule type="iconSet" priority="41">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="42">
       <iconSet iconSet="5Arrows">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="20"/>
@@ -3534,14 +3554,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16">
-    <cfRule type="iconSet" priority="35">
+    <cfRule type="iconSet" priority="39">
       <iconSet iconSet="3Symbols2">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
       </iconSet>
     </cfRule>
-    <cfRule type="iconSet" priority="36">
+    <cfRule type="iconSet" priority="40">
       <iconSet iconSet="3Symbols2">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -3550,14 +3570,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16">
-    <cfRule type="iconSet" priority="33">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="34">
+    <cfRule type="iconSet" priority="37">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="38">
       <iconSet iconSet="5Arrows">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="20"/>
@@ -3568,14 +3588,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="iconSet" priority="31">
+    <cfRule type="iconSet" priority="35">
       <iconSet iconSet="3Symbols2">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
       </iconSet>
     </cfRule>
-    <cfRule type="iconSet" priority="32">
+    <cfRule type="iconSet" priority="36">
       <iconSet iconSet="3Symbols2">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -3584,14 +3604,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H21">
-    <cfRule type="iconSet" priority="29">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="30">
+    <cfRule type="iconSet" priority="33">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="34">
       <iconSet iconSet="5Arrows">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="20"/>
@@ -3602,14 +3622,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="iconSet" priority="27">
+    <cfRule type="iconSet" priority="31">
       <iconSet iconSet="3Symbols2">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
       </iconSet>
     </cfRule>
-    <cfRule type="iconSet" priority="28">
+    <cfRule type="iconSet" priority="32">
       <iconSet iconSet="3Symbols2">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -3618,14 +3638,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H22">
-    <cfRule type="iconSet" priority="25">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="26">
+    <cfRule type="iconSet" priority="29">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="30">
       <iconSet iconSet="5Arrows">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="20"/>
@@ -3636,14 +3656,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="iconSet" priority="23">
+    <cfRule type="iconSet" priority="27">
       <iconSet iconSet="3Symbols2">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
       </iconSet>
     </cfRule>
-    <cfRule type="iconSet" priority="24">
+    <cfRule type="iconSet" priority="28">
       <iconSet iconSet="3Symbols2">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -3652,14 +3672,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="iconSet" priority="21">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="22">
+    <cfRule type="iconSet" priority="25">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="26">
       <iconSet iconSet="5Arrows">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="20"/>
@@ -3669,15 +3689,15 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J13">
-    <cfRule type="iconSet" priority="11">
+  <conditionalFormatting sqref="H18:H19">
+    <cfRule type="iconSet" priority="7">
       <iconSet iconSet="3Symbols2">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
       </iconSet>
     </cfRule>
-    <cfRule type="iconSet" priority="12">
+    <cfRule type="iconSet" priority="8">
       <iconSet iconSet="3Symbols2">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -3685,15 +3705,15 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J13">
-    <cfRule type="iconSet" priority="9">
-      <iconSet iconSet="3Symbols2" showValue="0">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-    <cfRule type="iconSet" priority="10">
+  <conditionalFormatting sqref="H18:H19">
+    <cfRule type="iconSet" priority="5">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+    <cfRule type="iconSet" priority="6">
       <iconSet iconSet="5Arrows">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="20"/>
@@ -3703,7 +3723,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H18:H19">
+  <conditionalFormatting sqref="J13">
     <cfRule type="iconSet" priority="3">
       <iconSet iconSet="3Symbols2">
         <cfvo type="percent" val="0"/>
@@ -3719,7 +3739,7 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H18:H19">
+  <conditionalFormatting sqref="J13">
     <cfRule type="iconSet" priority="1">
       <iconSet iconSet="3Symbols2" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -3757,14 +3777,14 @@
   </cols>
   <sheetData>
     <row r="5" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D5" s="51" t="s">
+      <c r="D5" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="54"/>
     </row>
     <row r="6" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D6" s="10" t="s">
@@ -3794,10 +3814,10 @@
         <v>7</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="H7" s="2">
         <v>1</v>
@@ -3809,7 +3829,7 @@
         <v>2</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="17" t="s">
@@ -3847,7 +3867,7 @@
         <v>0</v>
       </c>
       <c r="I10" s="15" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="4:9" x14ac:dyDescent="0.3">
@@ -3865,7 +3885,7 @@
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="15" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="H12" s="2">
         <v>1</v>
@@ -3879,7 +3899,7 @@
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
       <c r="G13" s="15" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="H13" s="2">
         <v>1</v>
@@ -3893,7 +3913,7 @@
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
       <c r="G14" s="15" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="H14" s="2">
         <v>1</v>
@@ -3907,7 +3927,7 @@
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
       <c r="G15" s="15" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="H15" s="2">
         <v>1</v>
@@ -3921,7 +3941,7 @@
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
       <c r="G16" s="15" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="H16" s="2">
         <v>1</v>
@@ -3935,13 +3955,13 @@
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
       <c r="G17" s="15" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="H17" s="2">
         <v>1</v>
       </c>
       <c r="I17" s="15" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="4:9" x14ac:dyDescent="0.3">
@@ -3951,7 +3971,7 @@
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
       <c r="G18" s="15" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H18" s="2">
         <v>1</v>
@@ -3965,7 +3985,7 @@
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
       <c r="G19" s="15" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="H19" s="2">
         <v>1</v>
@@ -3977,7 +3997,7 @@
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
       <c r="G20" s="15" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="H20" s="2">
         <v>1</v>
@@ -3997,7 +4017,7 @@
         <v>0</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="4:9" x14ac:dyDescent="0.3">
@@ -4015,7 +4035,7 @@
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
       <c r="G23" s="15" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="H23" s="2">
         <v>1</v>
@@ -4029,7 +4049,7 @@
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
       <c r="G24" s="15" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="H24" s="2">
         <v>1</v>
@@ -4043,7 +4063,7 @@
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
       <c r="G25" s="15" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="H25" s="2">
         <v>1</v>
@@ -4055,13 +4075,13 @@
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
       <c r="G26" s="15" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="H26" s="2">
         <v>1</v>
       </c>
       <c r="I26" s="15" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="4:9" x14ac:dyDescent="0.3">
@@ -4069,7 +4089,7 @@
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
       <c r="G27" s="15" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H27" s="2">
         <v>1</v>
@@ -4083,7 +4103,7 @@
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
       <c r="G28" s="15" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="H28" s="2">
         <v>1</v>
@@ -4118,7 +4138,7 @@
       </c>
       <c r="E31" s="9"/>
       <c r="G31" s="15" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="H31" s="2">
         <v>1</v>
@@ -4131,7 +4151,7 @@
       </c>
       <c r="E32" s="9"/>
       <c r="G32" s="15" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="H32" s="2">
         <v>1</v>
@@ -4144,7 +4164,7 @@
       </c>
       <c r="E33" s="9"/>
       <c r="G33" s="15" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="H33" s="2">
         <v>1</v>
@@ -4157,7 +4177,7 @@
       </c>
       <c r="E34" s="9"/>
       <c r="G34" s="15" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="H34" s="2">
         <v>1</v>
@@ -4176,7 +4196,7 @@
         <v>0</v>
       </c>
       <c r="I35" s="15" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="36" spans="4:9" x14ac:dyDescent="0.3">
@@ -4193,7 +4213,7 @@
       <c r="E37" s="9"/>
       <c r="F37" s="14"/>
       <c r="G37" s="25" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="H37" s="2">
         <v>1</v>
@@ -4207,7 +4227,7 @@
       <c r="E38" s="9"/>
       <c r="F38" s="14"/>
       <c r="G38" s="25" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="H38" s="2">
         <v>1</v>
@@ -4221,7 +4241,7 @@
       <c r="E39" s="9"/>
       <c r="F39" s="14"/>
       <c r="G39" s="25" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="H39" s="2">
         <v>1</v>
@@ -4235,7 +4255,7 @@
       <c r="E40" s="9"/>
       <c r="F40" s="14"/>
       <c r="G40" s="16" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="H40" s="2">
         <v>1</v>
@@ -4249,7 +4269,7 @@
       <c r="E41" s="9"/>
       <c r="F41" s="14"/>
       <c r="G41" s="25" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="H41" s="2">
         <v>1</v>
@@ -4263,7 +4283,7 @@
       <c r="E42" s="9"/>
       <c r="F42" s="14"/>
       <c r="G42" s="25" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="H42" s="2">
         <v>1</v>
@@ -4283,7 +4303,7 @@
         <v>0</v>
       </c>
       <c r="I43" s="15" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="44" spans="4:9" x14ac:dyDescent="0.3">
@@ -4300,7 +4320,7 @@
       <c r="E45" s="9"/>
       <c r="F45" s="14"/>
       <c r="G45" s="25" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="H45" s="2">
         <v>1</v>
@@ -4314,7 +4334,7 @@
       <c r="E46" s="9"/>
       <c r="F46" s="14"/>
       <c r="G46" s="25" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="H46" s="2">
         <v>1</v>
@@ -4328,7 +4348,7 @@
       <c r="E47" s="9"/>
       <c r="F47" s="14"/>
       <c r="G47" s="16" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="H47" s="2">
         <v>1</v>
@@ -4342,7 +4362,7 @@
       <c r="E48" s="9"/>
       <c r="F48" s="14"/>
       <c r="G48" s="16" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="H48" s="2">
         <v>1</v>
@@ -4356,7 +4376,7 @@
       <c r="E49" s="9"/>
       <c r="F49" s="14"/>
       <c r="G49" s="16" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="H49" s="2">
         <v>1</v>
@@ -4370,7 +4390,7 @@
       <c r="E50" s="9"/>
       <c r="F50" s="14"/>
       <c r="G50" s="25" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="H50" s="2">
         <v>1</v>
@@ -4390,7 +4410,7 @@
         <v>0</v>
       </c>
       <c r="I51" s="15" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="52" spans="4:9" x14ac:dyDescent="0.3">
@@ -4408,7 +4428,7 @@
       <c r="E53" s="9"/>
       <c r="F53" s="14"/>
       <c r="G53" s="25" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H53" s="2">
         <v>1</v>
@@ -4422,7 +4442,7 @@
       <c r="E54" s="9"/>
       <c r="F54" s="14"/>
       <c r="G54" s="25" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="H54" s="2">
         <v>1</v>
@@ -4436,7 +4456,7 @@
       <c r="E55" s="9"/>
       <c r="F55" s="14"/>
       <c r="G55" s="25" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="H55" s="2">
         <v>1</v>
@@ -4450,7 +4470,7 @@
       <c r="E56" s="9"/>
       <c r="F56" s="14"/>
       <c r="G56" s="16" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="H56" s="2">
         <v>1</v>
@@ -4470,7 +4490,7 @@
         <v>0</v>
       </c>
       <c r="I57" s="15" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="58" spans="4:9" x14ac:dyDescent="0.3">
@@ -4502,7 +4522,7 @@
       <c r="E60" s="9"/>
       <c r="F60" s="14"/>
       <c r="G60" s="25" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="H60" s="2">
         <v>1</v>
@@ -4516,7 +4536,7 @@
       <c r="E61" s="9"/>
       <c r="F61" s="14"/>
       <c r="G61" s="25" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="H61" s="2">
         <v>1</v>
@@ -4530,7 +4550,7 @@
       <c r="E62" s="9"/>
       <c r="F62" s="14"/>
       <c r="G62" s="16" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="H62" s="2">
         <v>1</v>
@@ -4544,7 +4564,7 @@
       <c r="E63" s="9"/>
       <c r="F63" s="14"/>
       <c r="G63" s="25" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="H63" s="2">
         <v>1</v>
@@ -4558,7 +4578,7 @@
       <c r="E64" s="9"/>
       <c r="F64" s="14"/>
       <c r="G64" s="25" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="H64" s="2">
         <v>1</v>
@@ -4572,7 +4592,7 @@
       <c r="E65" s="9"/>
       <c r="F65" s="14"/>
       <c r="G65" s="25" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="H65" s="2">
         <v>1</v>
@@ -4586,7 +4606,7 @@
       <c r="E66" s="9"/>
       <c r="F66" s="14"/>
       <c r="G66" s="25" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="H66" s="2">
         <v>1</v>
@@ -4606,7 +4626,7 @@
         <v>0</v>
       </c>
       <c r="I67" s="15" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="68" spans="4:9" x14ac:dyDescent="0.3">

</xml_diff>